<commit_message>
cambios y cat de tipo oficio
</commit_message>
<xml_diff>
--- a/public/reportes/informe.xlsx
+++ b/public/reportes/informe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Nombre:</t>
   </si>
@@ -65,12 +65,6 @@
     <t>FECHA VENCIMIENTO</t>
   </si>
   <si>
-    <t>ADMINISTRACIÓN DE OFICIOS:</t>
-  </si>
-  <si>
-    <t>SECRETARÍA</t>
-  </si>
-  <si>
     <t>UNIDAD ADMINISTRATIVA</t>
   </si>
   <si>
@@ -86,21 +80,12 @@
     <t>FECHA VENCIMENTO</t>
   </si>
   <si>
-    <t>NOTIFICACIONES:</t>
-  </si>
-  <si>
-    <t>CONTESTACIÓN ÓRGANO:</t>
-  </si>
-  <si>
     <t>PRÓRROGA</t>
   </si>
   <si>
     <t>Tipo de Auditoría:</t>
   </si>
   <si>
-    <t>ADMINISTRACIÓN DE RESULTADOS:</t>
-  </si>
-  <si>
     <t>TIPO DE RESULTADO</t>
   </si>
   <si>
@@ -120,6 +105,21 @@
   </si>
   <si>
     <t>NUMERO RESULTADO</t>
+  </si>
+  <si>
+    <t>ORDEN DE AUDITORÍA</t>
+  </si>
+  <si>
+    <t>NOTIFICACIÓN A ÁREAS</t>
+  </si>
+  <si>
+    <t>CONTESTACIÓN ÓRGANO FISCALIZADOR</t>
+  </si>
+  <si>
+    <t>ADMINISTRACIÓN DE RESULTADOS</t>
+  </si>
+  <si>
+    <t>TIPO OFICIO</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,11 +243,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,132 +569,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="4" max="4" width="33.7265625" customWidth="1"/>
+    <col min="2" max="3" width="22.1796875" customWidth="1"/>
     <col min="5" max="5" width="28.90625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.1796875" customWidth="1"/>
-    <col min="23" max="23" width="32.81640625" customWidth="1"/>
-    <col min="24" max="24" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.54296875" customWidth="1"/>
-    <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="29" max="29" width="12.1796875" customWidth="1"/>
-    <col min="30" max="30" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.08984375" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.36328125" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="19.36328125" customWidth="1"/>
+    <col min="16" max="17" width="20.90625" customWidth="1"/>
+    <col min="19" max="19" width="22" customWidth="1"/>
+    <col min="20" max="20" width="13.90625" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" customWidth="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.1796875" customWidth="1"/>
+    <col min="30" max="30" width="32.81640625" customWidth="1"/>
+    <col min="31" max="31" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="27.54296875" customWidth="1"/>
+    <col min="35" max="35" width="15" customWidth="1"/>
+    <col min="36" max="36" width="12.1796875" customWidth="1"/>
+    <col min="37" max="37" width="18.81640625" customWidth="1"/>
+    <col min="38" max="38" width="15.08984375" customWidth="1"/>
+    <col min="39" max="39" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="L9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="S9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="AA9" s="6" t="s">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="L9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="S9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Z9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AH9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
+      <c r="C10" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>7</v>
@@ -697,73 +715,92 @@
         <v>12</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="S10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="V10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S10" s="2" t="s">
+      <c r="X10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AH10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB10" s="3" t="s">
+      <c r="AI10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AJ10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AK10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AE10" s="5" t="s">
+      <c r="AL10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AF10" s="5" t="s">
+      <c r="AM10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="AA9:AF9"/>
+  <mergeCells count="6">
+    <mergeCell ref="AH9:AM9"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="S9:X9"/>
+    <mergeCell ref="Z9:AF9"/>
     <mergeCell ref="L9:Q9"/>
-    <mergeCell ref="S9:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>